<commit_message>
muitas mudanças de design
</commit_message>
<xml_diff>
--- a/src/assets/template_cadastro.xlsx
+++ b/src/assets/template_cadastro.xlsx
@@ -1,36 +1,58 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sucesso em Vendas\Python\Boopt\src\assets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF210CB-6A8B-4088-BBE5-F02472AB6D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="720" yWindow="1185" windowWidth="16305" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Cadastro" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>CPF</t>
+  </si>
+  <si>
+    <t>Data de Nascimento</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Cargo/Função</t>
+  </si>
+  <si>
+    <t>Nome completo</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="DD/MM/YYYY"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -49,97 +71,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Usuarios" displayName="Usuarios" ref="A1:F2" headerRowCount="1">
-  <autoFilter ref="A1:F2"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Primeiro Nome"/>
-    <tableColumn id="2" name="Sobrenome"/>
-    <tableColumn id="3" name="CPF"/>
-    <tableColumn id="4" name="Data de Nascimento"/>
-    <tableColumn id="5" name="Email"/>
-    <tableColumn id="6" name="Cargo/Função"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Usuarios" displayName="Usuarios" ref="A1:E2">
+  <autoFilter ref="A1:E2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Nome completo"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="CPF"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Data de Nascimento"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Email"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Cargo/Função"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -427,62 +389,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="32" customWidth="1" min="1" max="1"/>
-    <col width="32" customWidth="1" min="2" max="2"/>
-    <col width="16" customWidth="1" style="1" min="3" max="3"/>
-    <col width="16" customWidth="1" style="2" min="4" max="4"/>
-    <col width="32" customWidth="1" min="5" max="5"/>
-    <col width="16" customWidth="1" min="6" max="6"/>
+    <col min="1" max="1" width="32" customWidth="1"/>
+    <col min="2" max="2" width="16" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16" style="2" customWidth="1"/>
+    <col min="4" max="4" width="32" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Primeiro Nome</t>
-        </is>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Sobrenome</t>
-        </is>
+      <c r="B1" t="s">
+        <v>0</v>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>CPF</t>
-        </is>
+      <c r="C1" t="s">
+        <v>1</v>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Data de Nascimento</t>
-        </is>
+      <c r="D1" t="s">
+        <v>2</v>
       </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Cargo/Função</t>
-        </is>
+      <c r="E1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="F2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation type="list" allowBlank="1" sqref="E2" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Atendente,Diretor Comercial,Gerente de Loja,Regional,Supervisor de Loja,Vendedor"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
unidades, nova logo e alguns refatoramentos
</commit_message>
<xml_diff>
--- a/src/assets/template_cadastro.xlsx
+++ b/src/assets/template_cadastro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sucesso em Vendas\Python\Boopt\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF210CB-6A8B-4088-BBE5-F02472AB6D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C076159-1B19-4E5F-BFF8-B6DFC9205445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="1185" windowWidth="16305" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2430" yWindow="795" windowWidth="17715" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>CPF</t>
-  </si>
-  <si>
-    <t>Data de Nascimento</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Email</t>
   </si>
   <si>
-    <t>Cargo/Função</t>
-  </si>
-  <si>
-    <t>Nome completo</t>
+    <t>Nome completo*</t>
+  </si>
+  <si>
+    <t>CPF*</t>
+  </si>
+  <si>
+    <t>Data de Nascimento*</t>
+  </si>
+  <si>
+    <t>Cargo/Função*</t>
+  </si>
+  <si>
+    <t>Unidade(s)*</t>
   </si>
 </sst>
 </file>
@@ -70,15 +73,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -92,14 +100,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Usuarios" displayName="Usuarios" ref="A1:E2">
-  <autoFilter ref="A1:E2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Nome completo"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="CPF"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Data de Nascimento"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Usuarios" displayName="Usuarios" ref="A1:F2" insertRow="1">
+  <autoFilter ref="A1:F2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Nome completo*"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="CPF*"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Data de Nascimento*"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Email"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Cargo/Função"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Cargo/Função*"/>
+    <tableColumn id="2" xr3:uid="{115A938C-066F-45BD-B540-6E4F353ED0B7}" name="Unidade(s)*" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -390,36 +399,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
     <col min="2" max="2" width="16" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="2" customWidth="1"/>
+    <col min="3" max="3" width="26" style="2" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>